<commit_message>
1) loading data 2) validating data (partially) 3) introduced UUid
</commit_message>
<xml_diff>
--- a/loader/src/main/resources/CropClass.xlsx
+++ b/loader/src/main/resources/CropClass.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23507"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23524"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{99BEB440-79E7-4989-838A-D38FB2BC542A}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{16AFA440-4EEC-4CDF-8F56-B02743011A67}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -388,7 +388,7 @@
     <t>8d68d3c5-7b40-4588-b25e-4ea05527e1af</t>
   </si>
   <si>
-    <t>Other crops</t>
+    <t>Other crops2</t>
   </si>
 </sst>
 </file>
@@ -782,7 +782,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="E53" sqref="E53"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.42578125" defaultRowHeight="15"/>
   <cols>

</xml_diff>